<commit_message>
modificacion para los textos con espacios
</commit_message>
<xml_diff>
--- a/data/predicciones_grupo_16.xlsx
+++ b/data/predicciones_grupo_16.xlsx
@@ -6245,7 +6245,7 @@
         <v>1</v>
       </c>
       <c r="C447" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="448">
@@ -6466,7 +6466,7 @@
         <v>3</v>
       </c>
       <c r="C464" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="465">

</xml_diff>